<commit_message>
code binarysearch and array
</commit_message>
<xml_diff>
--- a/Problem - Practice-DSA.xlsx
+++ b/Problem - Practice-DSA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="6250" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="6250" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="solution" sheetId="3" r:id="rId6"/>
     <sheet name="Practice" sheetId="7" r:id="rId7"/>
     <sheet name="seanparshad" sheetId="8" r:id="rId8"/>
+    <sheet name="More practice" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="263">
   <si>
     <t>Srno</t>
   </si>
@@ -826,12 +827,18 @@
   <si>
     <t>with get n natural number sum and subtract with sum array element , second approach with XOR</t>
   </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/convert-array-into-zig-zag-fashion1638</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/find-the-odd-occurence4820</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,6 +872,12 @@
       <color rgb="FF212121"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="7">
@@ -918,7 +931,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -956,6 +969,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3290,7 +3306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3343,4 +3359,53 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="64.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update ds and decorator pattern
</commit_message>
<xml_diff>
--- a/Problem - Practice-DSA.xlsx
+++ b/Problem - Practice-DSA.xlsx
@@ -9,19 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="6250" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="6250" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="must_do" sheetId="6" r:id="rId2"/>
-    <sheet name="more problem" sheetId="4" r:id="rId3"/>
-    <sheet name="Behavour" sheetId="5" r:id="rId4"/>
-    <sheet name="Dout" sheetId="2" r:id="rId5"/>
-    <sheet name="solution" sheetId="3" r:id="rId6"/>
-    <sheet name="Practice" sheetId="7" r:id="rId7"/>
-    <sheet name="seanparshad" sheetId="8" r:id="rId8"/>
-    <sheet name="More practice" sheetId="9" r:id="rId9"/>
-    <sheet name="SDESkills" sheetId="10" r:id="rId10"/>
+    <sheet name="Githubrecord" sheetId="11" r:id="rId1"/>
+    <sheet name="Desgine pattern" sheetId="12" r:id="rId2"/>
+    <sheet name="System Degine" sheetId="15" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="must_do" sheetId="6" r:id="rId5"/>
+    <sheet name="more problem" sheetId="4" r:id="rId6"/>
+    <sheet name="Behavour" sheetId="5" r:id="rId7"/>
+    <sheet name="Dout" sheetId="2" r:id="rId8"/>
+    <sheet name="solution" sheetId="3" r:id="rId9"/>
+    <sheet name="Practice" sheetId="7" r:id="rId10"/>
+    <sheet name="seanparshad" sheetId="8" r:id="rId11"/>
+    <sheet name="More practice" sheetId="9" r:id="rId12"/>
+    <sheet name="SDESkills" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="318">
   <si>
     <t>Srno</t>
   </si>
@@ -843,12 +846,168 @@
   <si>
     <t>https://leetcode.com/problems/number-of-ways-to-wear-different-hats-to-each-other/</t>
   </si>
+  <si>
+    <t>Problem List</t>
+  </si>
+  <si>
+    <t>Attempt</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Remarkrs</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/activity-selection-1587115620/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/at-least-two-greater-elements4625/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/average4856/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/check-if-two-arrays-are-equal-or-not3847/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/compete-the-skills5807/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/convert-array-into-zig-zag-fashion1638/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/display-longest-name0853/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/find-the-odd-occurence4820/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/find-index4752/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/kadanes-algorithm-1587115620/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/maximum-repeating-number4858/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/perfect-arrays4645/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/print-alternate-elements-of-an-array/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/print-the-left-element2009/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/-rearrange-array-alternately-1587115620/1</t>
+  </si>
+  <si>
+    <t>Path github</t>
+  </si>
+  <si>
+    <t>DSASheet\Array-string\GeekForGeeks\</t>
+  </si>
+  <si>
+    <t>DSASheet\Recursion\</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/subset-sums2234/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/permutations-of-a-given-string-1587115620/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/shuffle-integers2401/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/power-of-numbers-1587115620/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/pascal-triangle0652/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/josephus-problem/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/second-largest3735/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/segregate-even-and-odd-numbers4629/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/smaller-and-larger4005/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/sort-an-array-of-0s-1s-and-2s4231/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/sum-of-array2326/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/third-largest-element/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/trapping-rain-water-1587115621/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/value-equal-to-index-value1330/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/all-numbers-with-specific-difference3558/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/ffd66b6a0bf7cefb9987fa455974b6ea5695709e/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/find-pair-given-difference1559/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/find-the-closest-number5513/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/first-and-last-occurrences-of-x2041/1</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/magical-number-1587115620/1</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>DSASheet\BinarySearch\</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decorator Pattern </t>
+  </si>
+  <si>
+    <t>Link1</t>
+  </si>
+  <si>
+    <t>Rate Limiter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,8 +1048,15 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -927,6 +1093,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -941,7 +1125,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -982,6 +1166,17 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1264,6 +1459,1307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="65.1796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="6" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.81640625" customWidth="1"/>
+    <col min="9" max="9" width="43.90625" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H1" s="20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H2" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H3" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>44830</v>
+      </c>
+      <c r="G7" s="7">
+        <f>F7+5</f>
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>44830</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" ref="G8:G45" si="0">F8+5</f>
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>44830</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <v>44831</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>44836</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>44831</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>44836</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
+        <v>44831</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>44836</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7">
+        <f>F20+5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>17</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="7">
+        <f>F26+5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C27" s="23"/>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="C29" s="23"/>
+      <c r="D29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>22</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>23</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C31" s="23"/>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>24</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32" s="23"/>
+      <c r="D32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C33" s="23"/>
+      <c r="D33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="G34" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="C35" s="23"/>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="G35" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="G36" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>29</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="C37" s="23"/>
+      <c r="D37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="G37" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G38" s="7">
+        <f>F38+5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B39" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="G39" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>30</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="C40" s="23"/>
+      <c r="D40" t="s">
+        <v>312</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" s="7">
+        <v>44831</v>
+      </c>
+      <c r="G40" s="7">
+        <f t="shared" si="0"/>
+        <v>44836</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>31</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" t="s">
+        <v>312</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>44831</v>
+      </c>
+      <c r="G41" s="7">
+        <f t="shared" si="0"/>
+        <v>44836</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>32</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="C42" s="23"/>
+      <c r="D42" t="s">
+        <v>312</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" s="7">
+        <v>44831</v>
+      </c>
+      <c r="G42" s="7">
+        <f t="shared" si="0"/>
+        <v>44836</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>33</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C43" s="23"/>
+      <c r="D43" t="s">
+        <v>312</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" s="7">
+        <v>44831</v>
+      </c>
+      <c r="G43" s="7">
+        <f t="shared" si="0"/>
+        <v>44836</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>34</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="C44" s="23"/>
+      <c r="D44" t="s">
+        <v>312</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" s="7">
+        <v>44831</v>
+      </c>
+      <c r="G44" s="7">
+        <f t="shared" si="0"/>
+        <v>44836</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>35</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="C45" s="23"/>
+      <c r="D45" t="s">
+        <v>312</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7">
+        <v>44831</v>
+      </c>
+      <c r="G45" s="7">
+        <f t="shared" si="0"/>
+        <v>44836</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B10" r:id="rId4"/>
+    <hyperlink ref="B11" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId6"/>
+    <hyperlink ref="B16" r:id="rId7"/>
+    <hyperlink ref="B18" r:id="rId8"/>
+    <hyperlink ref="B12" r:id="rId9"/>
+    <hyperlink ref="B17" r:id="rId10"/>
+    <hyperlink ref="B19" r:id="rId11"/>
+    <hyperlink ref="B20" r:id="rId12"/>
+    <hyperlink ref="B21" r:id="rId13"/>
+    <hyperlink ref="B22" r:id="rId14"/>
+    <hyperlink ref="B23" r:id="rId15"/>
+    <hyperlink ref="B24" r:id="rId16"/>
+    <hyperlink ref="B25" r:id="rId17"/>
+    <hyperlink ref="B26" r:id="rId18"/>
+    <hyperlink ref="B27" r:id="rId19"/>
+    <hyperlink ref="B28" r:id="rId20"/>
+    <hyperlink ref="B29" r:id="rId21"/>
+    <hyperlink ref="B30" r:id="rId22"/>
+    <hyperlink ref="B31" r:id="rId23"/>
+    <hyperlink ref="B32" r:id="rId24"/>
+    <hyperlink ref="B33" r:id="rId25"/>
+    <hyperlink ref="B34" r:id="rId26"/>
+    <hyperlink ref="B35" r:id="rId27"/>
+    <hyperlink ref="B36" r:id="rId28"/>
+    <hyperlink ref="B37" r:id="rId29"/>
+    <hyperlink ref="B40" r:id="rId30"/>
+    <hyperlink ref="B41" r:id="rId31"/>
+    <hyperlink ref="B42" r:id="rId32"/>
+    <hyperlink ref="B43" r:id="rId33"/>
+    <hyperlink ref="B44" r:id="rId34"/>
+    <hyperlink ref="B45" r:id="rId35"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="60.90625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="39.54296875" customWidth="1"/>
+    <col min="4" max="4" width="41.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="47.36328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="47.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="64.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="59.1796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="28.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="G1" s="20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="G2" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="G3" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>44833</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="23.90625" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="G1" s="20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="G2" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="G3" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2575,66 +4071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="59.1796875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
@@ -2933,7 +4370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C6"/>
   <sheetViews>
@@ -2995,7 +4432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B40"/>
   <sheetViews>
@@ -3198,7 +4635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C4"/>
   <sheetViews>
@@ -3240,7 +4677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3258,223 +4695,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="60.90625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="39.54296875" customWidth="1"/>
-    <col min="4" max="4" width="41.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="C5" t="s">
-        <v>249</v>
-      </c>
-      <c r="D5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>252</v>
-      </c>
-      <c r="D6" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>224</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
-    <hyperlink ref="A7" r:id="rId5"/>
-    <hyperlink ref="A8" r:id="rId6"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="47.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="47.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="64.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
-        <v>245</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-</worksheet>
 </file>
</xml_diff>